<commit_message>
corrected null cell value from ui
</commit_message>
<xml_diff>
--- a/CTDC_Automation/TestData/TC_Canine_Filter_1.xlsx
+++ b/CTDC_Automation/TestData/TC_Canine_Filter_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laxmi\KatalonApril24\DataCommons_Automation\CTDC_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Script\DataCommons_Automation\CTDC_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497A30C7-EE16-4EAC-8C38-BD0991F14EBD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86A6D25-A3E9-4D69-BC64-86F2792A4B35}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3645" yWindow="3105" windowWidth="12225" windowHeight="7815" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="testcase" sheetId="2" r:id="rId1"/>
@@ -310,9 +310,6 @@
     <t>Select_case_checkbox</t>
   </si>
   <si>
-    <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WITH DISTINCT c AS c, p, s, demo, diag RETURN c.case_id AS `Case ID`, s.clinical_study_designation AS `Study Code`, s.clinical_study_type AS `Study Type`, demo.breed AS Breed, diag.disease_term AS Diagnosis, diag.stage_of_disease AS `Stage of Disease`,demo.patient_age_at_enrollment AS Age, demo.sex AS Sex, demo.neutered_indicator AS `Neutered Status`</t>
-  </si>
-  <si>
     <t>compare</t>
   </si>
   <si>
@@ -331,9 +328,6 @@
     <t>G_rowcount</t>
   </si>
   <si>
-    <t>19</t>
-  </si>
-  <si>
     <t xml:space="preserve">Description </t>
   </si>
   <si>
@@ -377,6 +371,12 @@
   </si>
   <si>
     <t>bolt://ncias-s2261-c.nci.nih.gov:7687</t>
+  </si>
+  <si>
+    <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WITH DISTINCT c AS c, p, s, demo, diag RETURN c.case_id AS `Case ID`, s.clinical_study_designation AS `Study Code`, s.clinical_study_type AS `Study Type`, demo.breed AS Breed, diag.disease_term AS Diagnosis, coalesce(diag.stage_of_disease,'') AS `Stage of Disease`,demo.patient_age_at_enrollment AS Age, demo.sex AS Sex, coalesce(demo.neutered_indicator,'')  AS `Neutered Status`</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
 </sst>
 </file>
@@ -752,20 +752,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C468257-9521-42A0-A4DB-E0691FA7FE45}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="G3" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="76" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" customWidth="1"/>
-    <col min="7" max="7" width="99.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.7265625" customWidth="1"/>
+    <col min="7" max="7" width="99.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -800,7 +800,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -835,12 +835,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -855,7 +855,7 @@
         <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H3" t="s">
         <v>22</v>
@@ -870,7 +870,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -905,7 +905,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -925,7 +925,7 @@
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H5" t="s">
         <v>20</v>
@@ -940,7 +940,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -960,7 +960,7 @@
         <v>20</v>
       </c>
       <c r="G6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H6" t="s">
         <v>20</v>
@@ -975,7 +975,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1018,11 +1018,11 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" t="s">
         <v>97</v>
       </c>
-      <c r="D8" t="s">
-        <v>98</v>
-      </c>
       <c r="E8" t="s">
         <v>20</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>20</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="H8" t="s">
         <v>20</v>
@@ -1045,7 +1045,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>20</v>
       </c>
       <c r="I10" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="J10" t="s">
         <v>43</v>
@@ -1115,7 +1115,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>20</v>
       </c>
       <c r="J11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1165,72 +1165,72 @@
       <selection activeCell="B4" sqref="B4:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="79.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>100</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" t="s">
         <v>111</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C11" t="s">
-        <v>113</v>
       </c>
       <c r="D11" t="s">
         <v>29</v>
@@ -1239,47 +1239,47 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D26" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D27" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D28" t="s">
         <v>37</v>
       </c>
@@ -1287,12 +1287,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D29" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D31" t="s">
         <v>37</v>
       </c>
@@ -1300,27 +1300,27 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D33" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D35" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C38" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D39" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>1</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>1</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>1</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>1</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>1</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>1</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>1</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>1</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>1</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>1</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>20</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>1</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>1</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>20</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>1</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>1</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>1</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>1</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>1</v>
       </c>
@@ -2017,12 +2017,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C66" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C69" t="s">
         <v>77</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C70" t="s">
         <v>71</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C71" t="s">
         <v>80</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C72" t="s">
         <v>82</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C73" t="s">
         <v>74</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C74" t="s">
         <v>84</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C75" t="s">
         <v>86</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>1</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>1</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>1</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>1</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>1</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>20</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>20</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>20</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>20</v>
       </c>

</xml_diff>